<commit_message>
catch up from tuesday
</commit_message>
<xml_diff>
--- a/R_commands.xlsx
+++ b/R_commands.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonja\Documents\Dokumente\Studium\Master\Intro_to_programming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonja\OneDrive\Dokumente\EAGLE_Msc\Semester1\Intro_to_Programming\GitPractices\IntroToProgrammingPractices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6403980A-F71E-4519-9614-6918092B5B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C3CB5B-4DA6-4057-BE63-61D9BEB53905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{62FBD39C-FDE3-4025-952B-4860F9180D17}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{62FBD39C-FDE3-4025-952B-4860F9180D17}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="218">
   <si>
     <t>Action</t>
   </si>
@@ -654,13 +654,37 @@
     <t>Data Manipulation</t>
   </si>
   <si>
-    <t>Calculation</t>
-  </si>
-  <si>
     <t>Generation</t>
   </si>
   <si>
     <t>Spatial</t>
+  </si>
+  <si>
+    <t>Plot a sf object with ggplot2</t>
+  </si>
+  <si>
+    <t>ggplot()+geom_sf()</t>
+  </si>
+  <si>
+    <t>ggplot()+geom_sf(data=sfFile,fill=colour,color=outlineColour)</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>scale_y_continuous()</t>
+  </si>
+  <si>
+    <t>scale_fill_viridis_c()</t>
+  </si>
+  <si>
+    <t>Set the colour scale to viridis in a plot</t>
+  </si>
+  <si>
+    <t>scale_fill_viridis_c(option="A-H")</t>
+  </si>
+  <si>
+    <t>Position scales for continuous data</t>
   </si>
 </sst>
 </file>
@@ -1087,21 +1111,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA8AA0B-010E-4FE4-99E4-70D392929276}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.90625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="25.90625" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>190</v>
       </c>
@@ -1115,905 +1139,948 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>50</v>
+        <v>126</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>145</v>
+        <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>9</v>
+        <v>135</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>137</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>195</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>109</v>
+        <v>179</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>110</v>
+        <v>180</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>112</v>
+        <v>43</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>123</v>
+        <v>38</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>124</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>195</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>132</v>
+        <v>67</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
       <c r="D18" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>153</v>
+        <v>45</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>154</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>82</v>
+        <v>209</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>83</v>
+        <v>210</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>85</v>
+        <v>187</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>188</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>206</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>88</v>
+        <v>140</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D32" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D40" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D26" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D27" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D28" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D45" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B33" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C47" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D47" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D48" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D35" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
+      <c r="B49" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D36" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+      <c r="B50" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D50" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="D37" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D40" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D46" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D47" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="D48" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D50" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="B51" s="3" t="s">
-        <v>30</v>
+        <v>176</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>31</v>
+        <v>177</v>
       </c>
       <c r="D51" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>196</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>55</v>
+        <v>170</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>56</v>
+        <v>171</v>
       </c>
       <c r="D52" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>120</v>
+        <v>63</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>121</v>
+        <v>61</v>
       </c>
       <c r="D53" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>171</v>
+        <v>101</v>
       </c>
       <c r="D54" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>165</v>
+        <v>132</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D55" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>176</v>
+        <v>109</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>177</v>
+        <v>110</v>
       </c>
       <c r="D57" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>179</v>
+        <v>94</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>180</v>
+        <v>95</v>
       </c>
       <c r="D58" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>182</v>
+        <v>123</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+      <c r="D59" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>184</v>
+        <v>35</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>185</v>
+        <v>36</v>
       </c>
       <c r="D60" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D61" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D62" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D63" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="D64" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D65" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>118</v>
+        <v>8</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="D66" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>126</v>
+        <v>14</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>127</v>
+        <v>13</v>
       </c>
       <c r="D67" t="s">
-        <v>128</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D68" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D67" xr:uid="{EBA8AA0B-010E-4FE4-99E4-70D392929276}"/>
+  <autoFilter ref="A1:D67" xr:uid="{EBA8AA0B-010E-4FE4-99E4-70D392929276}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D68">
+      <sortCondition ref="C1:C67"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D67">
     <sortCondition ref="A1:A67"/>
   </sortState>

</xml_diff>